<commit_message>
script creates dataframe of oligos necessary for creating a triple gene ko
</commit_message>
<xml_diff>
--- a/template-paste-entry.xlsx
+++ b/template-paste-entry.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michaelvolk\Documents\repos\grna_scrape\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91E532BA-F479-4320-8573-2F963DAAA0CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F400634-E238-4B1F-8B84-99CB134327C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="5430" windowWidth="19440" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,6 +53,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -72,15 +77,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{F62FDF7D-68E6-477B-BF07-06B6714FDF8B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -395,18 +404,18 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="A2:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
     <col min="2" max="2" width="41.5703125" customWidth="1"/>
     <col min="3" max="3" width="10.140625" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>